<commit_message>
update mock for testing arbin sql db data to match new `from_arbin_to_datetime` function by @jayceslesar
</commit_message>
<xml_diff>
--- a/testdata/data/mock_data_001.xlsx
+++ b/testdata/data/mock_data_001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scripting\cellpy\testdata\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D677ECE-06B9-4A58-97F9-2A2CDCE2707A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFE4713E-3A51-4E41-AD37-484822443203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{498FF0A0-EEA8-4417-B1FF-B6433FCBEE83}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{498FF0A0-EEA8-4417-B1FF-B6433FCBEE83}"/>
   </bookViews>
   <sheets>
     <sheet name="arbin_sql" sheetId="2" r:id="rId1"/>
@@ -93,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="185" formatCode="0.0000000000000000000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000000000000000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -135,7 +135,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,23 +453,23 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C30"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="63.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1"/>
     <col min="14" max="14" width="24" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -519,7 +519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>22</v>
       </c>
@@ -527,8 +527,8 @@
         <v>12</v>
       </c>
       <c r="C2" s="2">
-        <f>1000000000000*(308400+(E2/(3600*24)))</f>
-        <v>3.0840000347222682E+17</v>
+        <f>16566949984405000+10000000*E2</f>
+        <v>1.6566952984409E+16</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -570,7 +570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>22</v>
       </c>
@@ -578,8 +578,8 @@
         <v>12</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C30" si="0">1000000000000*(308400+(E3/(3600*24)))</f>
-        <v>3.0840000694444794E+17</v>
+        <f>C2+10000000*E3</f>
+        <v>1.6566958984412E+16</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -621,7 +621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>22</v>
       </c>
@@ -629,8 +629,8 @@
         <v>12</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" si="0"/>
-        <v>3.0840001041667014E+17</v>
+        <f t="shared" ref="C4:C30" si="0">C3+10000000*E4</f>
+        <v>1.6566967984415E+16</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -672,7 +672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>22</v>
       </c>
@@ -681,7 +681,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
-        <v>3.084000138888912E+17</v>
+        <v>1.6566979984417E+16</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -723,7 +723,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>22</v>
       </c>
@@ -732,7 +732,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840001736111456E+17</v>
+        <v>1.656699498442E+16</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -774,7 +774,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>22</v>
       </c>
@@ -783,7 +783,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840002083333562E+17</v>
+        <v>1.6567012984422E+16</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -825,7 +825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>22</v>
       </c>
@@ -834,7 +834,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840002430555904E+17</v>
+        <v>1.6567033984425E+16</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -876,7 +876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>22</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840002777777773E+17</v>
+        <v>1.6567057984425E+16</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -927,7 +927,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>22</v>
       </c>
@@ -936,7 +936,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840003125E+17</v>
+        <v>1.6567084984425E+16</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -978,7 +978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>22</v>
       </c>
@@ -987,7 +987,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840003472222227E+17</v>
+        <v>1.6567114984425E+16</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1029,7 +1029,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>22</v>
       </c>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840003819444563E+17</v>
+        <v>1.6567147984426E+16</v>
       </c>
       <c r="D12">
         <v>11</v>
@@ -1080,7 +1080,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>22</v>
       </c>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004166667475E+17</v>
+        <v>1.6567183984433E+16</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -1131,7 +1131,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>22</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004166668288E+17</v>
+        <v>1.6567219984447E+16</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -1182,7 +1182,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>22</v>
       </c>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167335533E+17</v>
+        <v>1.6567255990226E+16</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -1233,7 +1233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>22</v>
       </c>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167351386E+17</v>
+        <v>1.6567291996142E+16</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -1284,7 +1284,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>22</v>
       </c>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167357408E+17</v>
+        <v>1.656732800211E+16</v>
       </c>
       <c r="D17">
         <v>16</v>
@@ -1335,7 +1335,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>22</v>
       </c>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167363194E+17</v>
+        <v>1.6567364008128E+16</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -1386,7 +1386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>22</v>
       </c>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167369907E+17</v>
+        <v>1.6567400014204E+16</v>
       </c>
       <c r="D19">
         <v>18</v>
@@ -1437,7 +1437,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>22</v>
       </c>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167377664E+17</v>
+        <v>1.6567436020347E+16</v>
       </c>
       <c r="D20">
         <v>19</v>
@@ -1488,7 +1488,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>22</v>
       </c>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" si="0"/>
-        <v>3.084000416738368E+17</v>
+        <v>1.6567472026542E+16</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -1539,7 +1539,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167396294E+17</v>
+        <v>1.6567508032846E+16</v>
       </c>
       <c r="D22">
         <v>21</v>
@@ -1590,7 +1590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167408685E+17</v>
+        <v>1.6567544039257E+16</v>
       </c>
       <c r="D23">
         <v>22</v>
@@ -1641,7 +1641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167422688E+17</v>
+        <v>1.6567580045789E+16</v>
       </c>
       <c r="D24">
         <v>23</v>
@@ -1692,7 +1692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>22</v>
       </c>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167435187E+17</v>
+        <v>1.6567616052429E+16</v>
       </c>
       <c r="D25">
         <v>24</v>
@@ -1743,7 +1743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="C26" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167447571E+17</v>
+        <v>1.6567652059176E+16</v>
       </c>
       <c r="D26">
         <v>25</v>
@@ -1794,7 +1794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>22</v>
       </c>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="C27" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167460531E+17</v>
+        <v>1.6567688066035E+16</v>
       </c>
       <c r="D27">
         <v>26</v>
@@ -1845,7 +1845,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>22</v>
       </c>
@@ -1854,7 +1854,7 @@
       </c>
       <c r="C28" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167473613E+17</v>
+        <v>1.6567724073007E+16</v>
       </c>
       <c r="D28">
         <v>27</v>
@@ -1896,7 +1896,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>22</v>
       </c>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="C29" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167486573E+17</v>
+        <v>1.6567760080091E+16</v>
       </c>
       <c r="D29">
         <v>28</v>
@@ -1947,7 +1947,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>22</v>
       </c>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="C30" s="2">
         <f t="shared" si="0"/>
-        <v>3.0840004167531827E+17</v>
+        <v>1.6567796087566E+16</v>
       </c>
       <c r="D30">
         <v>29</v>

</xml_diff>